<commit_message>
Revert "API 함수 개발#5"
This reverts commit 46d71990beeeaf578e3eac2a3fda38c19bd21d29.
</commit_message>
<xml_diff>
--- a/Assets/ItemDB.xlsx
+++ b/Assets/ItemDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hyeon\unityprojects\EarthDefenseCorps\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D3783-361F-4EBB-B00B-6CF753E6C9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2741BD0-1B33-447E-8A1B-E1F17DB9C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{891A0C57-32D1-4387-B303-CB8C03F152BC}"/>
+    <workbookView xWindow="780" yWindow="180" windowWidth="20835" windowHeight="11385" xr2:uid="{891A0C57-32D1-4387-B303-CB8C03F152BC}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDB" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="209">
   <si>
     <t>몽둥이</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,6 +50,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Epic</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unique</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Legendary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>데스사이드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -758,6 +778,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>itemSheldGager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>itemSpecialMoveGager</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -782,6 +806,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Legendary</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>Helmat</t>
+  </si>
+  <si>
+    <t>Sheld</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
     <t>itemGrade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -820,42 +865,6 @@
   <si>
     <t>철로 만들어진 기사의 갑주이다. 튼튼하지만 다소 무겁다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NORMAL</t>
-  </si>
-  <si>
-    <t>RARE</t>
-  </si>
-  <si>
-    <t>EPIC</t>
-  </si>
-  <si>
-    <t>UNIQUE</t>
-  </si>
-  <si>
-    <t>LEGENDARY</t>
-  </si>
-  <si>
-    <t>WEAPON</t>
-  </si>
-  <si>
-    <t>GLOVES</t>
-  </si>
-  <si>
-    <t>SHOES</t>
-  </si>
-  <si>
-    <t>itemSHIELDGager</t>
-  </si>
-  <si>
-    <t>SHIELD</t>
-  </si>
-  <si>
-    <t>HELMET</t>
-  </si>
-  <si>
-    <t>ARMOR</t>
   </si>
 </sst>
 </file>
@@ -1484,15 +1493,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7CCA2D-AB49-417B-A5BB-23E383A449C7}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="4" max="4" width="10.25" customWidth="1"/>
+    <col min="1" max="4" width="10.25" customWidth="1"/>
     <col min="5" max="5" width="16.875" customWidth="1"/>
     <col min="6" max="6" width="113.375" customWidth="1"/>
     <col min="7" max="7" width="10.25" customWidth="1"/>
@@ -1506,55 +1513,55 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>180</v>
-      </c>
       <c r="M1" s="12" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="Q1" s="13" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1562,10 +1569,10 @@
         <v>1000</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
@@ -1574,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G2" s="9">
         <v>2</v>
@@ -1615,10 +1622,10 @@
         <v>1001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1627,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G3" s="10">
         <v>3</v>
@@ -1668,10 +1675,10 @@
         <v>1002</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
@@ -1680,7 +1687,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G4" s="10">
         <v>4</v>
@@ -1721,19 +1728,19 @@
         <v>1003</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G5" s="10">
         <v>7</v>
@@ -1774,19 +1781,19 @@
         <v>1004</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G6" s="10">
         <v>10</v>
@@ -1827,19 +1834,19 @@
         <v>1005</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G7" s="10">
         <v>13</v>
@@ -1880,19 +1887,19 @@
         <v>1006</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G8" s="10">
         <v>25</v>
@@ -1933,19 +1940,19 @@
         <v>1007</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G9" s="10">
         <v>30</v>
@@ -1986,19 +1993,19 @@
         <v>1008</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G10" s="10">
         <v>35</v>
@@ -2039,19 +2046,19 @@
         <v>1009</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G11" s="10">
         <v>45</v>
@@ -2092,19 +2099,19 @@
         <v>1010</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G12" s="10">
         <v>50</v>
@@ -2145,19 +2152,19 @@
         <v>1011</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="G13" s="10">
         <v>55</v>
@@ -2198,19 +2205,19 @@
         <v>1012</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G14" s="10">
         <v>65</v>
@@ -2251,19 +2258,19 @@
         <v>1013</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G15" s="10">
         <v>70</v>
@@ -2304,19 +2311,19 @@
         <v>1014</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G16" s="10">
         <v>75</v>
@@ -2357,19 +2364,19 @@
         <v>2000</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -2410,19 +2417,19 @@
         <v>2001</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -2463,19 +2470,19 @@
         <v>2002</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -2516,19 +2523,19 @@
         <v>2003</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="G20" s="10">
         <v>1</v>
@@ -2569,19 +2576,19 @@
         <v>2004</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="G21" s="10">
         <v>3</v>
@@ -2622,19 +2629,19 @@
         <v>2005</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G22" s="10">
         <v>5</v>
@@ -2675,19 +2682,19 @@
         <v>2006</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G23" s="10">
         <v>5</v>
@@ -2728,19 +2735,19 @@
         <v>2007</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G24" s="10">
         <v>9</v>
@@ -2781,19 +2788,19 @@
         <v>2008</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G25" s="10">
         <v>13</v>
@@ -2834,19 +2841,19 @@
         <v>2009</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="G26" s="10">
         <v>13</v>
@@ -2887,19 +2894,19 @@
         <v>2010</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G27" s="10">
         <v>18</v>
@@ -2940,19 +2947,19 @@
         <v>2011</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="G28" s="10">
         <v>23</v>
@@ -2993,19 +3000,19 @@
         <v>2012</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G29" s="10">
         <v>23</v>
@@ -3046,19 +3053,19 @@
         <v>2013</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="G30" s="10">
         <v>30</v>
@@ -3099,19 +3106,19 @@
         <v>2014</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="G31" s="10">
         <v>37</v>
@@ -3152,19 +3159,19 @@
         <v>3000</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="G32" s="10">
         <v>1</v>
@@ -3205,19 +3212,19 @@
         <v>3001</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="G33" s="10">
         <v>2</v>
@@ -3258,19 +3265,19 @@
         <v>3002</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G34" s="10">
         <v>3</v>
@@ -3311,19 +3318,19 @@
         <v>3003</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G35" s="10">
         <v>3</v>
@@ -3364,19 +3371,19 @@
         <v>3004</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G36" s="10">
         <v>4</v>
@@ -3417,19 +3424,19 @@
         <v>3005</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G37" s="10">
         <v>5</v>
@@ -3470,19 +3477,19 @@
         <v>3006</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="G38" s="10">
         <v>5</v>
@@ -3523,19 +3530,19 @@
         <v>3007</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="G39" s="10">
         <v>9</v>
@@ -3576,19 +3583,19 @@
         <v>3008</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="G40" s="10">
         <v>13</v>
@@ -3629,19 +3636,19 @@
         <v>3009</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="G41" s="10">
         <v>13</v>
@@ -3682,19 +3689,19 @@
         <v>3010</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D42" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G42" s="10">
         <v>18</v>
@@ -3735,19 +3742,19 @@
         <v>3011</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="G43" s="10">
         <v>23</v>
@@ -3788,19 +3795,19 @@
         <v>3012</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="G44" s="10">
         <v>23</v>
@@ -3841,19 +3848,19 @@
         <v>3013</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="G45" s="10">
         <v>30</v>
@@ -3894,19 +3901,19 @@
         <v>3014</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D46" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G46" s="10">
         <v>37</v>
@@ -3947,19 +3954,19 @@
         <v>4000</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G47" s="4">
         <v>0</v>
@@ -4000,19 +4007,19 @@
         <v>4001</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G48" s="4">
         <v>0</v>
@@ -4053,19 +4060,19 @@
         <v>4002</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="G49" s="4">
         <v>0</v>
@@ -4106,19 +4113,19 @@
         <v>4003</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D50" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="G50" s="4">
         <v>0</v>
@@ -4159,19 +4166,19 @@
         <v>4004</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D51" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G51" s="4">
         <v>0</v>
@@ -4212,19 +4219,19 @@
         <v>4005</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D52" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="G52" s="4">
         <v>0</v>
@@ -4265,19 +4272,19 @@
         <v>4006</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D53" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G53" s="4">
         <v>0</v>
@@ -4318,19 +4325,19 @@
         <v>4007</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D54" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="G54" s="4">
         <v>0</v>
@@ -4371,19 +4378,19 @@
         <v>4008</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D55" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="G55" s="4">
         <v>0</v>
@@ -4424,19 +4431,19 @@
         <v>4009</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G56" s="4">
         <v>0</v>
@@ -4477,19 +4484,19 @@
         <v>4010</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D57" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="G57" s="4">
         <v>0</v>
@@ -4530,19 +4537,19 @@
         <v>4011</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D58" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="G58" s="4">
         <v>0</v>
@@ -4583,19 +4590,19 @@
         <v>4012</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D59" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="G59" s="4">
         <v>0</v>
@@ -4636,19 +4643,19 @@
         <v>4013</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G60" s="4">
         <v>0</v>
@@ -4689,19 +4696,19 @@
         <v>4014</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D61" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="G61" s="4">
         <v>0</v>
@@ -4742,19 +4749,19 @@
         <v>5000</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G62" s="4">
         <v>0</v>
@@ -4795,19 +4802,19 @@
         <v>5001</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D63" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="G63" s="4">
         <v>0</v>
@@ -4848,19 +4855,19 @@
         <v>5002</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="G64" s="4">
         <v>0</v>
@@ -4901,19 +4908,19 @@
         <v>5003</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="G65" s="4">
         <v>0</v>
@@ -4954,19 +4961,19 @@
         <v>5004</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G66" s="4">
         <v>0</v>
@@ -5007,19 +5014,19 @@
         <v>5005</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="G67" s="4">
         <v>0</v>
@@ -5060,19 +5067,19 @@
         <v>5006</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F68" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D68" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="G68" s="4">
         <v>0</v>
@@ -5113,19 +5120,19 @@
         <v>5007</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="G69" s="4">
         <v>0</v>
@@ -5166,19 +5173,19 @@
         <v>5008</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G70" s="4">
         <v>0</v>
@@ -5219,19 +5226,19 @@
         <v>5009</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D71" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="G71" s="4">
         <v>0</v>
@@ -5272,19 +5279,19 @@
         <v>5010</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D72" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="G72" s="4">
         <v>0</v>
@@ -5325,19 +5332,19 @@
         <v>5011</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="G73" s="4">
         <v>0</v>
@@ -5378,19 +5385,19 @@
         <v>5012</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="G74" s="4">
         <v>0</v>
@@ -5431,19 +5438,19 @@
         <v>5013</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G75" s="4">
         <v>0</v>
@@ -5484,19 +5491,19 @@
         <v>5014</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="G76" s="4">
         <v>0</v>
@@ -5537,19 +5544,19 @@
         <v>6000</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="G77" s="4">
         <v>0</v>
@@ -5590,19 +5597,19 @@
         <v>6001</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G78" s="4">
         <v>0</v>
@@ -5643,19 +5650,19 @@
         <v>6002</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>196</v>
+        <v>3</v>
       </c>
       <c r="D79" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="G79" s="4">
         <v>0</v>
@@ -5696,19 +5703,19 @@
         <v>6003</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D80" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="G80" s="4">
         <v>0</v>
@@ -5749,19 +5756,19 @@
         <v>6004</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>197</v>
+        <v>4</v>
       </c>
       <c r="D81" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="G81" s="4">
         <v>0</v>
@@ -5802,19 +5809,19 @@
         <v>6005</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="D82" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>194</v>
-      </c>
       <c r="F82" s="4" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="G82" s="4">
         <v>0</v>
@@ -5855,19 +5862,19 @@
         <v>6006</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D83" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="G83" s="4">
         <v>0</v>
@@ -5908,19 +5915,19 @@
         <v>6007</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D84" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="G84" s="4">
         <v>0</v>
@@ -5961,19 +5968,19 @@
         <v>6008</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="D85" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G85" s="4">
         <v>0</v>
@@ -6014,19 +6021,19 @@
         <v>6009</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G86" s="4">
         <v>0</v>
@@ -6067,19 +6074,19 @@
         <v>6010</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D87" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="G87" s="4">
         <v>0</v>
@@ -6120,19 +6127,19 @@
         <v>6011</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="D88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G88" s="4">
         <v>0</v>
@@ -6173,19 +6180,19 @@
         <v>6012</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="G89" s="4">
         <v>0</v>
@@ -6226,19 +6233,19 @@
         <v>6013</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>200</v>
+        <v>7</v>
       </c>
       <c r="D90" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G90" s="4">
         <v>0</v>
@@ -6279,19 +6286,19 @@
         <v>6014</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D91" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="G91" s="6">
         <v>0</v>
@@ -6333,11 +6340,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D91" xr:uid="{40D9CF25-DFAB-4524-9278-28B0DA711FA8}">
       <formula1>"FALSE, TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{311F0515-FC38-4118-BA6E-F726D3883E1F}">
-      <formula1>"NONE, NORMAL, RARE, EPIC, UNIQUE, LEGENDARY, COUNT"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C91" xr:uid="{1B28A208-8F52-458B-ADC7-6D2DFFB17C46}">
+      <formula1>"None, Normal, Rare, Epic, Unique, Legendary, Count"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{C2A726FE-33A9-422F-917D-0B5C7DC51BD0}">
-      <formula1>"NONE, WEAPON, GLOVES, SHOES, SHIELD, HELMET, ARMOR, COUNT"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B91" xr:uid="{CEB64A0E-4508-4A8C-93D3-E751161B7D47}">
+      <formula1>"None, Weapon, Gloves, Shoes, Sheld, Helmat, Armor, Count"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Revert "API 함수 개발#5""
This reverts commit 7eb145320ba02b1127ed75404ad87fce7259d2e4.
</commit_message>
<xml_diff>
--- a/Assets/ItemDB.xlsx
+++ b/Assets/ItemDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hyeon\unityprojects\EarthDefenseCorps\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2741BD0-1B33-447E-8A1B-E1F17DB9C342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D3783-361F-4EBB-B00B-6CF753E6C9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="180" windowWidth="20835" windowHeight="11385" xr2:uid="{891A0C57-32D1-4387-B303-CB8C03F152BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{891A0C57-32D1-4387-B303-CB8C03F152BC}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemDB" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="208">
   <si>
     <t>몽둥이</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,26 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rare</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Epic</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unique</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Legendary</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>데스사이드</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -778,10 +758,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>itemSheldGager</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>itemSpecialMoveGager</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -806,27 +782,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Legendary</t>
-  </si>
-  <si>
-    <t>Armor</t>
-  </si>
-  <si>
-    <t>Helmat</t>
-  </si>
-  <si>
-    <t>Sheld</t>
-  </si>
-  <si>
-    <t>Shoes</t>
-  </si>
-  <si>
-    <t>Gloves</t>
-  </si>
-  <si>
-    <t>Weapon</t>
-  </si>
-  <si>
     <t>itemGrade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -865,6 +820,42 @@
   <si>
     <t>철로 만들어진 기사의 갑주이다. 튼튼하지만 다소 무겁다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>RARE</t>
+  </si>
+  <si>
+    <t>EPIC</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>LEGENDARY</t>
+  </si>
+  <si>
+    <t>WEAPON</t>
+  </si>
+  <si>
+    <t>GLOVES</t>
+  </si>
+  <si>
+    <t>SHOES</t>
+  </si>
+  <si>
+    <t>itemSHIELDGager</t>
+  </si>
+  <si>
+    <t>SHIELD</t>
+  </si>
+  <si>
+    <t>HELMET</t>
+  </si>
+  <si>
+    <t>ARMOR</t>
   </si>
 </sst>
 </file>
@@ -1493,13 +1484,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7CCA2D-AB49-417B-A5BB-23E383A449C7}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.25" customWidth="1"/>
+    <col min="1" max="2" width="10.25" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
     <col min="5" max="5" width="16.875" customWidth="1"/>
     <col min="6" max="6" width="113.375" customWidth="1"/>
     <col min="7" max="7" width="10.25" customWidth="1"/>
@@ -1513,55 +1506,55 @@
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="K1" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="O1" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="P1" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="Q1" s="13" t="s">
         <v>185</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="M1" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1569,10 +1562,10 @@
         <v>1000</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D2" s="2" t="b">
         <v>0</v>
@@ -1581,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G2" s="9">
         <v>2</v>
@@ -1622,10 +1615,10 @@
         <v>1001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
@@ -1634,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G3" s="10">
         <v>3</v>
@@ -1675,10 +1668,10 @@
         <v>1002</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D4" s="2" t="b">
         <v>0</v>
@@ -1687,7 +1680,7 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G4" s="10">
         <v>4</v>
@@ -1728,19 +1721,19 @@
         <v>1003</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G5" s="10">
         <v>7</v>
@@ -1781,19 +1774,19 @@
         <v>1004</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G6" s="10">
         <v>10</v>
@@ -1834,19 +1827,19 @@
         <v>1005</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G7" s="10">
         <v>13</v>
@@ -1887,19 +1880,19 @@
         <v>1006</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G8" s="10">
         <v>25</v>
@@ -1940,19 +1933,19 @@
         <v>1007</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G9" s="10">
         <v>30</v>
@@ -1993,19 +1986,19 @@
         <v>1008</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="F10" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G10" s="10">
         <v>35</v>
@@ -2046,19 +2039,19 @@
         <v>1009</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G11" s="10">
         <v>45</v>
@@ -2099,19 +2092,19 @@
         <v>1010</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G12" s="10">
         <v>50</v>
@@ -2152,19 +2145,19 @@
         <v>1011</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G13" s="10">
         <v>55</v>
@@ -2205,19 +2198,19 @@
         <v>1012</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G14" s="10">
         <v>65</v>
@@ -2258,19 +2251,19 @@
         <v>1013</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G15" s="10">
         <v>70</v>
@@ -2311,19 +2304,19 @@
         <v>1014</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G16" s="10">
         <v>75</v>
@@ -2364,19 +2357,19 @@
         <v>2000</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -2417,19 +2410,19 @@
         <v>2001</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -2470,19 +2463,19 @@
         <v>2002</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -2523,19 +2516,19 @@
         <v>2003</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G20" s="10">
         <v>1</v>
@@ -2576,19 +2569,19 @@
         <v>2004</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G21" s="10">
         <v>3</v>
@@ -2629,19 +2622,19 @@
         <v>2005</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G22" s="10">
         <v>5</v>
@@ -2682,19 +2675,19 @@
         <v>2006</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G23" s="10">
         <v>5</v>
@@ -2735,19 +2728,19 @@
         <v>2007</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G24" s="10">
         <v>9</v>
@@ -2788,19 +2781,19 @@
         <v>2008</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G25" s="10">
         <v>13</v>
@@ -2841,19 +2834,19 @@
         <v>2009</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G26" s="10">
         <v>13</v>
@@ -2894,19 +2887,19 @@
         <v>2010</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G27" s="10">
         <v>18</v>
@@ -2947,19 +2940,19 @@
         <v>2011</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G28" s="10">
         <v>23</v>
@@ -3000,19 +2993,19 @@
         <v>2012</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G29" s="10">
         <v>23</v>
@@ -3053,19 +3046,19 @@
         <v>2013</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D30" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G30" s="10">
         <v>30</v>
@@ -3106,19 +3099,19 @@
         <v>2014</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D31" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G31" s="10">
         <v>37</v>
@@ -3159,19 +3152,19 @@
         <v>3000</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D32" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G32" s="10">
         <v>1</v>
@@ -3212,19 +3205,19 @@
         <v>3001</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D33" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G33" s="10">
         <v>2</v>
@@ -3265,19 +3258,19 @@
         <v>3002</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="D34" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G34" s="10">
         <v>3</v>
@@ -3318,19 +3311,19 @@
         <v>3003</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D35" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G35" s="10">
         <v>3</v>
@@ -3371,19 +3364,19 @@
         <v>3004</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D36" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G36" s="10">
         <v>4</v>
@@ -3424,19 +3417,19 @@
         <v>3005</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D37" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G37" s="10">
         <v>5</v>
@@ -3477,19 +3470,19 @@
         <v>3006</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D38" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G38" s="10">
         <v>5</v>
@@ -3530,19 +3523,19 @@
         <v>3007</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D39" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G39" s="10">
         <v>9</v>
@@ -3583,19 +3576,19 @@
         <v>3008</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D40" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G40" s="10">
         <v>13</v>
@@ -3636,19 +3629,19 @@
         <v>3009</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D41" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G41" s="10">
         <v>13</v>
@@ -3689,19 +3682,19 @@
         <v>3010</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D42" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G42" s="10">
         <v>18</v>
@@ -3742,19 +3735,19 @@
         <v>3011</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D43" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G43" s="10">
         <v>23</v>
@@ -3795,19 +3788,19 @@
         <v>3012</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D44" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G44" s="10">
         <v>23</v>
@@ -3848,19 +3841,19 @@
         <v>3013</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D45" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G45" s="10">
         <v>30</v>
@@ -3901,19 +3894,19 @@
         <v>3014</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D46" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G46" s="10">
         <v>37</v>
@@ -3954,19 +3947,19 @@
         <v>4000</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D47" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G47" s="4">
         <v>0</v>
@@ -4007,19 +4000,19 @@
         <v>4001</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D48" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G48" s="4">
         <v>0</v>
@@ -4060,19 +4053,19 @@
         <v>4002</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D49" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G49" s="4">
         <v>0</v>
@@ -4113,19 +4106,19 @@
         <v>4003</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D50" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G50" s="4">
         <v>0</v>
@@ -4166,19 +4159,19 @@
         <v>4004</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D51" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G51" s="4">
         <v>0</v>
@@ -4219,19 +4212,19 @@
         <v>4005</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D52" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="G52" s="4">
         <v>0</v>
@@ -4272,19 +4265,19 @@
         <v>4006</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D53" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G53" s="4">
         <v>0</v>
@@ -4325,19 +4318,19 @@
         <v>4007</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D54" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G54" s="4">
         <v>0</v>
@@ -4378,19 +4371,19 @@
         <v>4008</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D55" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G55" s="4">
         <v>0</v>
@@ -4431,19 +4424,19 @@
         <v>4009</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D56" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G56" s="4">
         <v>0</v>
@@ -4484,19 +4477,19 @@
         <v>4010</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D57" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G57" s="4">
         <v>0</v>
@@ -4537,19 +4530,19 @@
         <v>4011</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D58" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G58" s="4">
         <v>0</v>
@@ -4590,19 +4583,19 @@
         <v>4012</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D59" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G59" s="4">
         <v>0</v>
@@ -4643,19 +4636,19 @@
         <v>4013</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D60" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G60" s="4">
         <v>0</v>
@@ -4696,19 +4689,19 @@
         <v>4014</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D61" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G61" s="4">
         <v>0</v>
@@ -4749,19 +4742,19 @@
         <v>5000</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D62" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G62" s="4">
         <v>0</v>
@@ -4802,19 +4795,19 @@
         <v>5001</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D63" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G63" s="4">
         <v>0</v>
@@ -4855,19 +4848,19 @@
         <v>5002</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D64" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G64" s="4">
         <v>0</v>
@@ -4908,19 +4901,19 @@
         <v>5003</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D65" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="G65" s="4">
         <v>0</v>
@@ -4961,19 +4954,19 @@
         <v>5004</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D66" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G66" s="4">
         <v>0</v>
@@ -5014,19 +5007,19 @@
         <v>5005</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D67" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G67" s="4">
         <v>0</v>
@@ -5067,19 +5060,19 @@
         <v>5006</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D68" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="G68" s="4">
         <v>0</v>
@@ -5120,19 +5113,19 @@
         <v>5007</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D69" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G69" s="4">
         <v>0</v>
@@ -5173,19 +5166,19 @@
         <v>5008</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D70" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G70" s="4">
         <v>0</v>
@@ -5226,19 +5219,19 @@
         <v>5009</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D71" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G71" s="4">
         <v>0</v>
@@ -5279,19 +5272,19 @@
         <v>5010</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D72" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G72" s="4">
         <v>0</v>
@@ -5332,19 +5325,19 @@
         <v>5011</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D73" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G73" s="4">
         <v>0</v>
@@ -5385,19 +5378,19 @@
         <v>5012</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D74" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G74" s="4">
         <v>0</v>
@@ -5438,19 +5431,19 @@
         <v>5013</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D75" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G75" s="4">
         <v>0</v>
@@ -5491,19 +5484,19 @@
         <v>5014</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D76" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G76" s="4">
         <v>0</v>
@@ -5544,19 +5537,19 @@
         <v>6000</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D77" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G77" s="4">
         <v>0</v>
@@ -5597,19 +5590,19 @@
         <v>6001</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D78" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G78" s="4">
         <v>0</v>
@@ -5650,19 +5643,19 @@
         <v>6002</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>3</v>
+        <v>196</v>
       </c>
       <c r="D79" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G79" s="4">
         <v>0</v>
@@ -5703,19 +5696,19 @@
         <v>6003</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D80" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G80" s="4">
         <v>0</v>
@@ -5756,19 +5749,19 @@
         <v>6004</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D81" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G81" s="4">
         <v>0</v>
@@ -5809,19 +5802,19 @@
         <v>6005</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>4</v>
+        <v>197</v>
       </c>
       <c r="D82" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="G82" s="4">
         <v>0</v>
@@ -5862,19 +5855,19 @@
         <v>6006</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D83" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G83" s="4">
         <v>0</v>
@@ -5915,19 +5908,19 @@
         <v>6007</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D84" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G84" s="4">
         <v>0</v>
@@ -5968,19 +5961,19 @@
         <v>6008</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>5</v>
+        <v>198</v>
       </c>
       <c r="D85" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G85" s="4">
         <v>0</v>
@@ -6021,19 +6014,19 @@
         <v>6009</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D86" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G86" s="4">
         <v>0</v>
@@ -6074,19 +6067,19 @@
         <v>6010</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D87" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G87" s="4">
         <v>0</v>
@@ -6127,19 +6120,19 @@
         <v>6011</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>6</v>
+        <v>199</v>
       </c>
       <c r="D88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G88" s="4">
         <v>0</v>
@@ -6180,19 +6173,19 @@
         <v>6012</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D89" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G89" s="4">
         <v>0</v>
@@ -6233,19 +6226,19 @@
         <v>6013</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>7</v>
+        <v>200</v>
       </c>
       <c r="D90" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G90" s="4">
         <v>0</v>
@@ -6286,19 +6279,19 @@
         <v>6014</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D91" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G91" s="6">
         <v>0</v>
@@ -6340,11 +6333,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D91" xr:uid="{40D9CF25-DFAB-4524-9278-28B0DA711FA8}">
       <formula1>"FALSE, TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C91" xr:uid="{1B28A208-8F52-458B-ADC7-6D2DFFB17C46}">
-      <formula1>"None, Normal, Rare, Epic, Unique, Legendary, Count"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{311F0515-FC38-4118-BA6E-F726D3883E1F}">
+      <formula1>"NONE, NORMAL, RARE, EPIC, UNIQUE, LEGENDARY, COUNT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B91" xr:uid="{CEB64A0E-4508-4A8C-93D3-E751161B7D47}">
-      <formula1>"None, Weapon, Gloves, Shoes, Sheld, Helmat, Armor, Count"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{C2A726FE-33A9-422F-917D-0B5C7DC51BD0}">
+      <formula1>"NONE, WEAPON, GLOVES, SHOES, SHIELD, HELMET, ARMOR, COUNT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>